<commit_message>
interface overhual and check funcitons done
</commit_message>
<xml_diff>
--- a/samples/BiliBili_comments.xlsx
+++ b/samples/BiliBili_comments.xlsx
@@ -8,15 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hwang/Desktop/repo/VisualDTA/samples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED427456-320F-A84C-89E7-AE167382C042}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F5BD7E9-41AA-0B47-8E5C-71F179F81E4D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41040" yWindow="1220" windowWidth="30240" windowHeight="20380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19220" yWindow="500" windowWidth="19200" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$B$1:$B$2688</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -25,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="170">
   <si>
     <t>Proposition</t>
   </si>
@@ -156,36 +169,12 @@
     <t>h1</t>
   </si>
   <si>
-    <t>Q比特1903</t>
-  </si>
-  <si>
-    <t>unkown</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>正经人谁看评论区</t>
-  </si>
-  <si>
-    <t>2021-01-09 07:15</t>
-  </si>
-  <si>
-    <t>秀啊兄弟</t>
-  </si>
-  <si>
     <t>2021-01-09 07:45</t>
   </si>
   <si>
     <t>不清楚，随便找的</t>
   </si>
   <si>
-    <t>建议凉风</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
     <t>2021-01-09 07:46</t>
   </si>
   <si>
@@ -339,15 +328,6 @@
     <t>西天团里面没有一个不靠谱的小兄弟[doge]</t>
   </si>
   <si>
-    <t>陈畅小四C</t>
-  </si>
-  <si>
-    <t>2021-01-10 11:13</t>
-  </si>
-  <si>
-    <t>整的好</t>
-  </si>
-  <si>
     <t>折月桂光</t>
   </si>
   <si>
@@ -378,15 +358,6 @@
     <t>谢谢</t>
   </si>
   <si>
-    <t>狮驼国三大王</t>
-  </si>
-  <si>
-    <t>2021-01-11 17:31</t>
-  </si>
-  <si>
-    <t>自带川蜀口音[doge]</t>
-  </si>
-  <si>
     <t>瓦尔未遂</t>
   </si>
   <si>
@@ -396,15 +367,6 @@
     <t>[墨镜]</t>
   </si>
   <si>
-    <t>这个ID不需要硬币</t>
-  </si>
-  <si>
-    <t>2021-01-12 06:57</t>
-  </si>
-  <si>
-    <t>我tm[doge]哈哈哈哈</t>
-  </si>
-  <si>
     <t>云水斋主人</t>
   </si>
   <si>
@@ -414,15 +376,6 @@
     <t>also  know as可以理解为又名 别称 嘻哈中常见 放在歌曲开头或者结尾 主要是让大家记住自己的昵称或者tag</t>
   </si>
   <si>
-    <t>莫莫格湿地的小草</t>
-  </si>
-  <si>
-    <t>2021-01-14 04:14</t>
-  </si>
-  <si>
-    <t>EI YO 这里是AKA取精团，三个徒弟都是妖精男，路上把那妖精玩，用说唱炸的你胃痉挛[偷笑]</t>
-  </si>
-  <si>
     <t>Liiipxx</t>
   </si>
   <si>
@@ -486,15 +439,6 @@
     <t>爷是男的</t>
   </si>
   <si>
-    <t>阿祖不只是Dentist</t>
-  </si>
-  <si>
-    <t>2021-01-17 01:29</t>
-  </si>
-  <si>
-    <t>这里是大唐gang  来自东土大唐，西天文化靠我发扬，经历九九八十一难全员脸色蜡黄</t>
-  </si>
-  <si>
     <t>莫名厨大姐的大姐厨</t>
   </si>
   <si>
@@ -574,6 +518,36 @@
   </si>
   <si>
     <t>卐AKA.归西天团卍</t>
+  </si>
+  <si>
+    <t>Danmu discourse</t>
+  </si>
+  <si>
+    <t>Comment discourse</t>
+  </si>
+  <si>
+    <t>T(0)</t>
+  </si>
+  <si>
+    <t>P(1)</t>
+  </si>
+  <si>
+    <t>P(2)</t>
+  </si>
+  <si>
+    <t>P(3)</t>
+  </si>
+  <si>
+    <t>B(4)</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>danmus</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -609,7 +583,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -623,6 +597,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -962,10 +937,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H63"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A34" zoomScale="132" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="75" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1315,46 +1290,46 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B14" s="1" t="s">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="D14" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>45</v>
+      <c r="E14" s="1">
+        <v>10</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="G14" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>12</v>
-      </c>
-      <c r="B15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>42</v>
+      <c r="E15" s="1">
+        <v>11</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>12</v>
@@ -1368,19 +1343,19 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>13</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>8</v>
+        <v>14</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="C16" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="E16" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>12</v>
@@ -1394,45 +1369,45 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>14</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>8</v>
+        <v>15</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>11</v>
+        <v>52</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="G17" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>15</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>8</v>
+        <v>16</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E18" s="1">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>12</v>
@@ -1446,16 +1421,16 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E19" s="1">
         <v>0</v>
@@ -1472,16 +1447,16 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E20" s="1">
         <v>0</v>
@@ -1498,19 +1473,19 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E21" s="1">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>12</v>
@@ -1524,25 +1499,25 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E22" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="G22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22" s="1">
         <v>0</v>
@@ -1550,19 +1525,19 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E23" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>12</v>
@@ -1571,21 +1546,21 @@
         <v>0</v>
       </c>
       <c r="H23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E24" s="1">
         <v>11</v>
@@ -1602,25 +1577,25 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E25" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="G25" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H25" s="1">
         <v>0</v>
@@ -1628,10 +1603,10 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>23</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>76</v>
+        <v>24</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>77</v>
@@ -1640,7 +1615,7 @@
         <v>78</v>
       </c>
       <c r="E26" s="1">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>12</v>
@@ -1654,7 +1629,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>79</v>
@@ -1666,7 +1641,7 @@
         <v>81</v>
       </c>
       <c r="E27" s="1">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>12</v>
@@ -1680,7 +1655,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>82</v>
@@ -1692,13 +1667,13 @@
         <v>84</v>
       </c>
       <c r="E28" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="G28" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H28" s="1">
         <v>0</v>
@@ -1706,19 +1681,19 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <v>26</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>8</v>
+        <v>27</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E29" s="1">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>12</v>
@@ -1727,30 +1702,30 @@
         <v>0</v>
       </c>
       <c r="H29" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E30" s="1">
-        <v>25</v>
+        <v>90</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="G30" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H30" s="1">
         <v>0</v>
@@ -1758,10 +1733,10 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>90</v>
+        <v>36</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>91</v>
@@ -1770,13 +1745,13 @@
         <v>92</v>
       </c>
       <c r="E31" s="1">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="G31" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H31" s="1">
         <v>0</v>
@@ -1784,7 +1759,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>93</v>
@@ -1796,13 +1771,13 @@
         <v>95</v>
       </c>
       <c r="E32" s="1">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="G32" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H32" s="1">
         <v>0</v>
@@ -1810,7 +1785,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>96</v>
@@ -1821,8 +1796,8 @@
       <c r="D33" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E33" s="1" t="s">
-        <v>42</v>
+      <c r="E33" s="1">
+        <v>11</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>31</v>
@@ -1836,19 +1811,19 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>36</v>
+        <v>99</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E34" s="1">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>12</v>
@@ -1862,10 +1837,10 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <v>32</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>101</v>
+        <v>33</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>102</v>
@@ -1874,13 +1849,13 @@
         <v>103</v>
       </c>
       <c r="E35" s="1">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="G35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H35" s="1">
         <v>0</v>
@@ -1888,19 +1863,19 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C36" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="D36" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D36" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>42</v>
+      <c r="E36" s="1">
+        <v>36</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>12</v>
@@ -1914,25 +1889,25 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C37" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="D37" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D37" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="E37" s="1">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>31</v>
       </c>
       <c r="G37" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H37" s="1">
         <v>0</v>
@@ -1940,19 +1915,19 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C38" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="D38" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D38" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="E38" s="1">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>12</v>
@@ -1966,10 +1941,10 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <v>36</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>8</v>
+        <v>37</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>112</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>113</v>
@@ -1978,7 +1953,7 @@
         <v>114</v>
       </c>
       <c r="E39" s="1">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>12</v>
@@ -1992,25 +1967,25 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E40" s="1">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="G40" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H40" s="1">
         <v>0</v>
@@ -2018,10 +1993,10 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>117</v>
+        <v>8</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>118</v>
@@ -2029,14 +2004,14 @@
       <c r="D41" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="E41" s="1" t="s">
-        <v>42</v>
+      <c r="E41" s="1">
+        <v>44</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="G41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H41" s="1">
         <v>0</v>
@@ -2044,7 +2019,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>120</v>
@@ -2056,13 +2031,13 @@
         <v>122</v>
       </c>
       <c r="E42" s="1">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>31</v>
       </c>
       <c r="G42" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H42" s="1">
         <v>0</v>
@@ -2070,7 +2045,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>123</v>
@@ -2081,14 +2056,14 @@
       <c r="D43" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E43" s="1" t="s">
-        <v>42</v>
+      <c r="E43" s="1">
+        <v>0</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="G43" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H43" s="1">
         <v>0</v>
@@ -2096,25 +2071,25 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B44" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="D44" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="D44" s="1" t="s">
-        <v>128</v>
-      </c>
       <c r="E44" s="1">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="G44" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H44" s="1">
         <v>0</v>
@@ -2122,51 +2097,51 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C45" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="D45" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="D45" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>42</v>
+      <c r="E45" s="1">
+        <v>0</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="G45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B46" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C46" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>134</v>
-      </c>
       <c r="E46" s="1">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="G46" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H46" s="1">
         <v>0</v>
@@ -2174,25 +2149,25 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B47" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C47" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>137</v>
-      </c>
       <c r="E47" s="1">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="G47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H47" s="1">
         <v>0</v>
@@ -2200,25 +2175,25 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>8</v>
+        <v>136</v>
       </c>
       <c r="C48" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D48" s="1" t="s">
-        <v>139</v>
-      </c>
       <c r="E48" s="1">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="G48" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H48" s="1">
         <v>0</v>
@@ -2226,19 +2201,19 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C49" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="D49" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="D49" s="1" t="s">
-        <v>142</v>
-      </c>
       <c r="E49" s="1">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>31</v>
@@ -2252,25 +2227,25 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B50" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C50" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="D50" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D50" s="1" t="s">
-        <v>145</v>
-      </c>
       <c r="E50" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="G50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H50" s="1">
         <v>0</v>
@@ -2278,10 +2253,10 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>146</v>
@@ -2290,13 +2265,13 @@
         <v>147</v>
       </c>
       <c r="E51" s="1">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="G51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H51" s="1">
         <v>0</v>
@@ -2304,7 +2279,7 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>148</v>
@@ -2330,19 +2305,19 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>8</v>
+        <v>151</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E53" s="1">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>31</v>
@@ -2356,42 +2331,42 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>42</v>
+        <v>156</v>
+      </c>
+      <c r="E54" s="1">
+        <v>0</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>31</v>
       </c>
       <c r="G54" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H54" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E55" s="1">
         <v>0</v>
@@ -2406,220 +2381,983 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" s="1">
-        <v>53</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="E56" s="1">
-        <v>0</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G56" s="1">
-        <v>1</v>
-      </c>
-      <c r="H56" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A57" s="1">
-        <v>54</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="E57" s="1">
-        <v>4</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G57" s="1">
-        <v>1</v>
-      </c>
-      <c r="H57" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A58" s="1">
-        <v>55</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="E58" s="1">
-        <v>9</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G58" s="1">
-        <v>0</v>
-      </c>
-      <c r="H58" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A59" s="1">
-        <v>56</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="E59" s="1">
-        <v>0</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G59" s="1">
-        <v>0</v>
-      </c>
-      <c r="H59" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" s="1">
-        <v>57</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="E60" s="1">
-        <v>0</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G60" s="1">
-        <v>0</v>
-      </c>
-      <c r="H60" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A61" s="1">
-        <v>58</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="E61" s="1">
-        <v>19</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G61" s="1">
-        <v>1</v>
-      </c>
-      <c r="H61" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A62" s="1">
-        <v>59</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="E62" s="1">
-        <v>0</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G62" s="1">
-        <v>2</v>
-      </c>
-      <c r="H62" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" s="1">
-        <v>60</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="E63" s="1">
-        <v>0</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G63" s="1">
-        <v>0</v>
-      </c>
-      <c r="H63" s="1">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0ECECE4-541C-9B46-84AE-E5ED16241F36}">
+  <dimension ref="A1:N132"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>162</v>
+      </c>
+      <c r="F11" t="s">
+        <v>163</v>
+      </c>
+      <c r="H11" t="s">
+        <v>164</v>
+      </c>
+      <c r="J11" t="s">
+        <v>165</v>
+      </c>
+      <c r="L11" t="s">
+        <v>166</v>
+      </c>
+      <c r="N11" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>161</v>
+      </c>
+      <c r="D12">
+        <v>35</v>
+      </c>
+      <c r="E12" s="5">
+        <f>35/61</f>
+        <v>0.57377049180327866</v>
+      </c>
+      <c r="F12">
+        <v>19</v>
+      </c>
+      <c r="G12" s="5">
+        <f>19/61</f>
+        <v>0.31147540983606559</v>
+      </c>
+      <c r="H12">
+        <v>4</v>
+      </c>
+      <c r="I12" s="5">
+        <f>4/61</f>
+        <v>6.5573770491803282E-2</v>
+      </c>
+      <c r="J12">
+        <v>2</v>
+      </c>
+      <c r="K12" s="5">
+        <f>2/61</f>
+        <v>3.2786885245901641E-2</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12" s="5">
+        <f>1/61</f>
+        <v>1.6393442622950821E-2</v>
+      </c>
+      <c r="N12">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>160</v>
+      </c>
+      <c r="D13">
+        <v>32</v>
+      </c>
+      <c r="E13" s="5">
+        <f>32/130</f>
+        <v>0.24615384615384617</v>
+      </c>
+      <c r="F13">
+        <v>70</v>
+      </c>
+      <c r="G13" s="5">
+        <f>70/130</f>
+        <v>0.53846153846153844</v>
+      </c>
+      <c r="H13">
+        <v>23</v>
+      </c>
+      <c r="I13" s="5">
+        <f>23/131</f>
+        <v>0.17557251908396945</v>
+      </c>
+      <c r="J13">
+        <v>4</v>
+      </c>
+      <c r="K13" s="5">
+        <f>4/130</f>
+        <v>3.0769230769230771E-2</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13" s="5">
+        <f>1/130</f>
+        <v>7.6923076923076927E-3</v>
+      </c>
+      <c r="N13">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>4</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>0</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>0</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>0</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>0</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>0</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>1</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>0</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>0</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>0</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>0</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>0</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>3</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>0</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>1</v>
+      </c>
+      <c r="B33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>0</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>1</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>0</v>
+      </c>
+      <c r="B36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>1</v>
+      </c>
+      <c r="B37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>0</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>0</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>0</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>1</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>2</v>
+      </c>
+      <c r="B42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>0</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>0</v>
+      </c>
+      <c r="B44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <v>1</v>
+      </c>
+      <c r="B45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <v>0</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <v>1</v>
+      </c>
+      <c r="B47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>0</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>1</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <v>1</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>1</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>0</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <v>1</v>
+      </c>
+      <c r="B53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>1</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <v>0</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <v>1</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <v>1</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <v>0</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <v>0</v>
+      </c>
+      <c r="B59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
+        <v>0</v>
+      </c>
+      <c r="B60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
+        <v>1</v>
+      </c>
+      <c r="B61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <v>2</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
+        <v>0</v>
+      </c>
+      <c r="B63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B76">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B81">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B85">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B89">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B98">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B99">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B101">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="102" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B108">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="109" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B109">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B112">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B114">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="115" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B117">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B119">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B121">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B123">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B124">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B125">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B126">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B127">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B129">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="130" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B131">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="132" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B132">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
This version has basically all the functions.
</commit_message>
<xml_diff>
--- a/samples/BiliBili_comments.xlsx
+++ b/samples/BiliBili_comments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hwang/Desktop/repo/VisualDTA/samples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F5BD7E9-41AA-0B47-8E5C-71F179F81E4D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F761B3BB-7A66-8745-9948-90833D0A57A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19220" yWindow="500" windowWidth="19200" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="168">
   <si>
     <t>Proposition</t>
   </si>
@@ -175,6 +175,9 @@
     <t>不清楚，随便找的</t>
   </si>
   <si>
+    <t>B</t>
+  </si>
+  <si>
     <t>2021-01-09 07:46</t>
   </si>
   <si>
@@ -304,21 +307,6 @@
     <t>as know as,</t>
   </si>
   <si>
-    <t>铅笔刀_pencilknife</t>
-  </si>
-  <si>
-    <t>2021-01-10 08:10</t>
-  </si>
-  <si>
-    <t>好家伙，三连音都会整了</t>
-  </si>
-  <si>
-    <t>2021-01-10 08:16</t>
-  </si>
-  <si>
-    <t>好的👌</t>
-  </si>
-  <si>
     <t>吹箫吴市换龙衣</t>
   </si>
   <si>
@@ -548,6 +536,12 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>s34</t>
   </si>
 </sst>
 </file>
@@ -937,10 +931,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H55"/>
+  <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="75" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -991,16 +985,16 @@
         <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>11</v>
+        <v>166</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>166</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>11</v>
+        <v>166</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -1186,8 +1180,8 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>8</v>
+      <c r="A10" s="1" t="s">
+        <v>167</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>13</v>
@@ -1323,10 +1317,10 @@
         <v>8</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E15" s="1">
         <v>11</v>
@@ -1346,13 +1340,13 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E16" s="1">
         <v>0</v>
@@ -1372,13 +1366,13 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E17" s="1">
         <v>0</v>
@@ -1398,13 +1392,13 @@
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E18" s="1">
         <v>0</v>
@@ -1424,13 +1418,13 @@
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E19" s="1">
         <v>0</v>
@@ -1450,13 +1444,13 @@
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E20" s="1">
         <v>0</v>
@@ -1476,13 +1470,13 @@
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E21" s="1">
         <v>11</v>
@@ -1502,13 +1496,13 @@
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E22" s="1">
         <v>4</v>
@@ -1524,17 +1518,17 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="1">
-        <v>21</v>
+      <c r="A23" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E23" s="1">
         <v>10</v>
@@ -1554,13 +1548,13 @@
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E24" s="1">
         <v>11</v>
@@ -1580,13 +1574,13 @@
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E25" s="1">
         <v>0</v>
@@ -1609,13 +1603,13 @@
         <v>8</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E26" s="1">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>12</v>
@@ -1632,16 +1626,16 @@
         <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E27" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>12</v>
@@ -1658,13 +1652,13 @@
         <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E28" s="1">
         <v>10</v>
@@ -1684,13 +1678,13 @@
         <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E29" s="1">
         <v>11</v>
@@ -1707,19 +1701,19 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>42</v>
+        <v>91</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>31</v>
@@ -1733,25 +1727,25 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>36</v>
+        <v>92</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E31" s="1">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="G31" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H31" s="1">
         <v>0</v>
@@ -1759,25 +1753,25 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E32" s="1">
         <v>0</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="G32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H32" s="1">
         <v>0</v>
@@ -1785,25 +1779,25 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
-        <v>31</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>96</v>
+        <v>33</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E33" s="1">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="G33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H33" s="1">
         <v>0</v>
@@ -1811,10 +1805,10 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>100</v>
@@ -1823,7 +1817,7 @@
         <v>101</v>
       </c>
       <c r="E34" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>12</v>
@@ -1837,25 +1831,25 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <v>33</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>8</v>
+        <v>35</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>102</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E35" s="1">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="G35" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H35" s="1">
         <v>0</v>
@@ -1863,25 +1857,25 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E36" s="1">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="G36" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H36" s="1">
         <v>0</v>
@@ -1889,25 +1883,25 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E37" s="1">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="G37" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H37" s="1">
         <v>0</v>
@@ -1915,25 +1909,25 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E38" s="1">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="G38" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H38" s="1">
         <v>0</v>
@@ -1941,19 +1935,19 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>112</v>
+        <v>8</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E39" s="1">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>12</v>
@@ -1967,19 +1961,19 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E40" s="1">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>31</v>
@@ -1993,25 +1987,25 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>8</v>
+        <v>119</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E41" s="1">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="G41" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H41" s="1">
         <v>0</v>
@@ -2019,19 +2013,19 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E42" s="1">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>31</v>
@@ -2045,25 +2039,25 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E43" s="1">
         <v>0</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="G43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H43" s="1">
         <v>0</v>
@@ -2071,19 +2065,19 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>115</v>
+        <v>8</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="E44" s="1">
-        <v>45</v>
+        <v>128</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>167</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>31</v>
@@ -2097,16 +2091,16 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E45" s="1">
         <v>0</v>
@@ -2123,19 +2117,19 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>8</v>
+        <v>132</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E46" s="1">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>31</v>
@@ -2149,25 +2143,25 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E47" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="G47" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H47" s="1">
         <v>0</v>
@@ -2175,25 +2169,25 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="E48" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="G48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H48" s="1">
         <v>0</v>
@@ -2201,25 +2195,25 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="E49" s="1">
-        <v>4</v>
+        <v>143</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="G49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H49" s="1">
         <v>0</v>
@@ -2227,19 +2221,19 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E50" s="1">
-        <v>9</v>
+        <v>146</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>12</v>
@@ -2253,25 +2247,25 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="E51" s="1">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="G51" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H51" s="1">
         <v>0</v>
@@ -2279,25 +2273,25 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="E52" s="1">
         <v>0</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="G52" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H52" s="1">
         <v>0</v>
@@ -2305,79 +2299,27 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E53" s="1">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="G53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H53" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="1">
-        <v>52</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="E54" s="1">
-        <v>0</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G54" s="1">
-        <v>2</v>
-      </c>
-      <c r="H54" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A55" s="1">
-        <v>53</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="E55" s="1">
-        <v>0</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G55" s="1">
-        <v>0</v>
-      </c>
-      <c r="H55" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2410,10 +2352,10 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
@@ -2496,22 +2438,22 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
+        <v>158</v>
+      </c>
+      <c r="F11" t="s">
+        <v>159</v>
+      </c>
+      <c r="H11" t="s">
+        <v>160</v>
+      </c>
+      <c r="J11" t="s">
+        <v>161</v>
+      </c>
+      <c r="L11" t="s">
         <v>162</v>
       </c>
-      <c r="F11" t="s">
-        <v>163</v>
-      </c>
-      <c r="H11" t="s">
-        <v>164</v>
-      </c>
-      <c r="J11" t="s">
+      <c r="N11" t="s">
         <v>165</v>
-      </c>
-      <c r="L11" t="s">
-        <v>166</v>
-      </c>
-      <c r="N11" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
@@ -2522,7 +2464,7 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D12">
         <v>35</v>
@@ -2571,7 +2513,7 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D13">
         <v>32</v>

</xml_diff>

<commit_message>
alpha 2.0 new features
1. yellow square 1st propostion 2. x-axis forever integrer 3. mean semantic distance with only Ps 4.Breaks are not associated with other nodes
Todo:X-Y propotionality and hover effects
</commit_message>
<xml_diff>
--- a/samples/BiliBili_comments.xlsx
+++ b/samples/BiliBili_comments.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hwang/Desktop/repo/VisualDTA/samples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F761B3BB-7A66-8745-9948-90833D0A57A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A1A61DD-EA65-0343-A9B0-2466222873EE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19220" yWindow="500" windowWidth="19200" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6680" yWindow="500" windowWidth="31720" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$F$1:$F$53</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$B$1:$B$2688</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -934,7 +935,7 @@
   <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="75" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1869,7 +1870,7 @@
         <v>107</v>
       </c>
       <c r="E36" s="1">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>45</v>
@@ -1895,7 +1896,7 @@
         <v>110</v>
       </c>
       <c r="E37" s="1">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>45</v>

</xml_diff>